<commit_message>
adding some more PBI criteria
</commit_message>
<xml_diff>
--- a/docs/WorkPackageManagement_PBI.xlsx
+++ b/docs/WorkPackageManagement_PBI.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="139">
   <si>
     <t>BackLog Items</t>
   </si>
@@ -398,6 +398,54 @@
   </si>
   <si>
     <t>End user should be able to navigate and access the application with the help of this document</t>
+  </si>
+  <si>
+    <t>Admin user should be able to create new roles in system</t>
+  </si>
+  <si>
+    <t>Admin user should be able to update exising roles in application</t>
+  </si>
+  <si>
+    <t>Admin user should be able to view list roles in system</t>
+  </si>
+  <si>
+    <t>Admin user should be able to create new Users for system</t>
+  </si>
+  <si>
+    <t>Admin user should be able to modify existing users in system</t>
+  </si>
+  <si>
+    <t>Admin user should be able to view list of users along with their status in system</t>
+  </si>
+  <si>
+    <t>Admin user should be able to assign /unassign roles to user</t>
+  </si>
+  <si>
+    <t>Admin user should be able to add new resource type in system using some UI interface</t>
+  </si>
+  <si>
+    <t>Admin user should be able to modify resource type in system using some UI interface</t>
+  </si>
+  <si>
+    <t>Admin user should be able to update exisitng applications information in system using UI internface</t>
+  </si>
+  <si>
+    <t>Admin user should be able to create new applications in system using UI interface</t>
+  </si>
+  <si>
+    <t>Admin user should be able to associate rates with resource types using some UI interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin user should be able to associate user with ApplicationGroup role to the application </t>
+  </si>
+  <si>
+    <t>Demand management group user should be able to edit information about existing work package</t>
+  </si>
+  <si>
+    <t>Upon saving of WorkPackage the application should already send email notification for each WorkRequest to the user associate with Application</t>
+  </si>
+  <si>
+    <t>Application group user should be able to edit information about existing work request</t>
   </si>
 </sst>
 </file>
@@ -1016,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
@@ -1026,7 +1074,7 @@
     <col min="2" max="2" width="13.85546875" customWidth="1"/>
     <col min="3" max="3" width="6.5703125" customWidth="1"/>
     <col min="4" max="4" width="69.42578125" customWidth="1"/>
-    <col min="5" max="5" width="31" customWidth="1"/>
+    <col min="5" max="5" width="62.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="35" customWidth="1"/>
     <col min="7" max="16" width="6.5703125" customWidth="1"/>
     <col min="17" max="26" width="13.28515625" customWidth="1"/>
@@ -2310,7 +2358,7 @@
       <c r="Y36" s="2"/>
       <c r="Z36" s="2"/>
     </row>
-    <row r="37" spans="1:26">
+    <row r="37" spans="1:26" ht="26.25">
       <c r="A37" s="3" t="s">
         <v>61</v>
       </c>
@@ -2323,7 +2371,9 @@
       <c r="D37" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E37" s="4"/>
+      <c r="E37" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="F37" s="1"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
@@ -2346,7 +2396,7 @@
       <c r="Y37" s="2"/>
       <c r="Z37" s="2"/>
     </row>
-    <row r="38" spans="1:26">
+    <row r="38" spans="1:26" ht="26.25">
       <c r="A38" s="3" t="s">
         <v>63</v>
       </c>
@@ -2359,7 +2409,9 @@
       <c r="D38" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E38" s="4"/>
+      <c r="E38" s="4" t="s">
+        <v>124</v>
+      </c>
       <c r="F38" s="1"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
@@ -2382,7 +2434,7 @@
       <c r="Y38" s="2"/>
       <c r="Z38" s="2"/>
     </row>
-    <row r="39" spans="1:26">
+    <row r="39" spans="1:26" ht="26.25">
       <c r="A39" s="3" t="s">
         <v>65</v>
       </c>
@@ -2395,7 +2447,9 @@
       <c r="D39" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E39" s="4"/>
+      <c r="E39" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="F39" s="1"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
@@ -2418,7 +2472,7 @@
       <c r="Y39" s="2"/>
       <c r="Z39" s="2"/>
     </row>
-    <row r="40" spans="1:26">
+    <row r="40" spans="1:26" ht="26.25">
       <c r="A40" s="3" t="s">
         <v>67</v>
       </c>
@@ -2431,7 +2485,9 @@
       <c r="D40" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E40" s="4"/>
+      <c r="E40" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F40" s="1"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
@@ -2454,7 +2510,7 @@
       <c r="Y40" s="2"/>
       <c r="Z40" s="2"/>
     </row>
-    <row r="41" spans="1:26">
+    <row r="41" spans="1:26" ht="26.25">
       <c r="A41" s="3" t="s">
         <v>69</v>
       </c>
@@ -2467,7 +2523,9 @@
       <c r="D41" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E41" s="4"/>
+      <c r="E41" s="4" t="s">
+        <v>127</v>
+      </c>
       <c r="F41" s="1"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
@@ -2490,7 +2548,7 @@
       <c r="Y41" s="2"/>
       <c r="Z41" s="2"/>
     </row>
-    <row r="42" spans="1:26">
+    <row r="42" spans="1:26" ht="39">
       <c r="A42" s="3" t="s">
         <v>71</v>
       </c>
@@ -2503,7 +2561,9 @@
       <c r="D42" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E42" s="4"/>
+      <c r="E42" s="4" t="s">
+        <v>128</v>
+      </c>
       <c r="F42" s="1"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
@@ -2526,7 +2586,7 @@
       <c r="Y42" s="2"/>
       <c r="Z42" s="2"/>
     </row>
-    <row r="43" spans="1:26">
+    <row r="43" spans="1:26" ht="26.25">
       <c r="A43" s="3" t="s">
         <v>73</v>
       </c>
@@ -2539,7 +2599,9 @@
       <c r="D43" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E43" s="4"/>
+      <c r="E43" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="F43" s="1"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
@@ -2575,7 +2637,9 @@
       <c r="D44" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E44" s="4"/>
+      <c r="E44" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="F44" s="1"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
@@ -2611,7 +2675,9 @@
       <c r="D45" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E45" s="4"/>
+      <c r="E45" s="4" t="s">
+        <v>131</v>
+      </c>
       <c r="F45" s="1"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
@@ -2647,7 +2713,9 @@
       <c r="D46" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E46" s="4"/>
+      <c r="E46" s="4" t="s">
+        <v>134</v>
+      </c>
       <c r="F46" s="1"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
@@ -2670,7 +2738,7 @@
       <c r="Y46" s="2"/>
       <c r="Z46" s="2"/>
     </row>
-    <row r="47" spans="1:26">
+    <row r="47" spans="1:26" ht="26.25">
       <c r="A47" s="6" t="s">
         <v>81</v>
       </c>
@@ -2683,7 +2751,9 @@
       <c r="D47" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E47" s="4"/>
+      <c r="E47" s="4" t="s">
+        <v>133</v>
+      </c>
       <c r="F47" s="1"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
@@ -2706,7 +2776,7 @@
       <c r="Y47" s="2"/>
       <c r="Z47" s="2"/>
     </row>
-    <row r="48" spans="1:26">
+    <row r="48" spans="1:26" ht="39">
       <c r="A48" s="6" t="s">
         <v>83</v>
       </c>
@@ -2719,7 +2789,9 @@
       <c r="D48" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E48" s="4"/>
+      <c r="E48" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="F48" s="1"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
@@ -2755,7 +2827,9 @@
       <c r="D49" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E49" s="4"/>
+      <c r="E49" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="F49" s="1"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
@@ -2791,7 +2865,9 @@
       <c r="D50" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E50" s="4"/>
+      <c r="E50" s="4" t="s">
+        <v>136</v>
+      </c>
       <c r="F50" s="1"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
@@ -2827,7 +2903,9 @@
       <c r="D51" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E51" s="4"/>
+      <c r="E51" s="4" t="s">
+        <v>137</v>
+      </c>
       <c r="F51" s="1"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
@@ -2863,7 +2941,9 @@
       <c r="D52" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E52" s="4"/>
+      <c r="E52" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="F52" s="1"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>

</xml_diff>